<commit_message>
powerSource link to MotAs
</commit_message>
<xml_diff>
--- a/flag/AQB_classification/powerSource/powerSource_notes_was_flag_OTUs_v2.xlsx
+++ b/flag/AQB_classification/powerSource/powerSource_notes_was_flag_OTUs_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmat471/HD/GitHub/bioinfRhints/flag/AQB_classification/powerSource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3DB46F-C0EF-5447-8752-703BEAD12CDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E38B71A-09D3-7447-A621-F4E3308D204E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33100" yWindow="660" windowWidth="32600" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3320" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3557" uniqueCount="1547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3928" uniqueCount="1644">
   <si>
     <t>Table S4. Species Analyzed In The Study.</t>
   </si>
@@ -4667,13 +4667,313 @@
   </si>
   <si>
     <t>Baccillus trypoxylicola</t>
+  </si>
+  <si>
+    <t>Bacillus pseudofirmus</t>
+  </si>
+  <si>
+    <t>MotA_tr_tipname</t>
+  </si>
+  <si>
+    <t>MotB_original</t>
+  </si>
+  <si>
+    <t>tr|Q65KJ0|Q65KJ0_BACLD Motility protein B OS=Bacillus licheniformis (strain ATCC 14580 / DSM 13 / JCM 2505 / NBRC 12200 / NCIMB 9375 / NRRL NRS-1264 / Gibson 46) OX=279010 GN=motB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|T0P6Y4|T0P6Y4_AERSA Flagellar motor protein MotB OS=Aeromonas salmonicida subsp. pectinolytica 34mel OX=1324960 GN=motB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>sp|P28612|MOTB_BACSU Motility protein B OS=Bacillus subtilis (strain 168) OX=224308 GN=motB PE=3 SV=1</t>
+  </si>
+  <si>
+    <t>tr|A0A0S2SCT2|A0A0S2SCT2_9GAMM Flagellar motor protein MotB OS=Aeromonas schubertii OX=652 GN=motB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|C4XPD2|C4XPD2_DESMR Chemotaxis protein MotB OS=Desulfovibrio magneticus (strain ATCC 700980 / DSM 13731 / RS-1) OX=573370 GN=motB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>sp|P0AF06|MOTB_ECOLI Motility protein B OS=Escherichia coli (strain K12) OX=83333 GN=motB PE=1 SV=1</t>
+  </si>
+  <si>
+    <t>tr|Q5KWX0|Q5KWX0_GEOKA Motility protein B (Flagellar motor rotation) OS=Geobacillus kaustophilus (strain HTA426) OX=235909 GN=motB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>sp|P56427|MOTB_HELPY Motility protein B OS=Helicobacter pylori (strain ATCC 700392 / 26695) OX=85962 GN=motB PE=1 SV=1</t>
+  </si>
+  <si>
+    <t>tr|Q8CX95|Q8CX95_OCEIH Motility protein B (Flagellar motor rotation) OS=Oceanobacillus iheyensis (strain DSM 14371 / CIP 107618 / JCM 11309 / KCTC 3954 / HTE831) OX=221109 GN=OB2544 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|Q9HUL2|Q9HUL2_PSEAE Chemotaxis protein MotB OS=Pseudomonas aeruginosa (strain ATCC 15692 / DSM 22644 / CIP 104116 / JCM 14847 / LMG 12228 / 1C / PRS 101 / PAO1) OX=208964 GN=motB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>sp|Q53174|MOTA_RHOSH Motility protein A OS=Rhodobacter sphaeroides OX=1063 GN=motA PE=3 SV=1</t>
+  </si>
+  <si>
+    <t>sp|P55892|MOTB_SALTY Motility protein B OS=Salmonella typhimurium (strain LT2 / SGSC1412 / ATCC 700720) OX=99287 GN=motB PE=1 SV=1</t>
+  </si>
+  <si>
+    <t>tr|A0A0E8TCW6|A0A0E8TCW6_STREE Chemotaxis protein MotB OS=Streptococcus pneumoniae OX=1313 GN=motB_1 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|A0A0T8PK69|A0A0T8PK69_STREE Chemotaxis protein MotB OS=Streptococcus pneumoniae OX=1313 GN=motB_2 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|G4FDE7|G4FDE7_THEMA Flagellar motor rotation protein MotB OS=Thermotoga maritima (strain ATCC 43589 / MSB8 / DSM 3109 / JCM 10099) OX=243274 GN=Tmari_0677 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|A0A0M1V6Y6|A0A0M1V6Y6_YERPE Chemotaxis MotB protein OS=Yersinia pestis biovar Orientalis str. IP275 OX=373665 GN=motB1 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|B9KAV2|B9KAV2_THENN Motility protein B OS=Thermotoga neapolitana (strain ATCC 49049 / DSM 4359 / NS-E) OX=309803 GN=CTN_1909 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|Q5WGI6|Q5WGI6_BACSK Motility protein B OS=Bacillus clausii (strain KSM-K16) OX=66692 GN=motB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|B0SK95|B0SK95_LEPBP Chemotaxis MotB protein OS=Leptospira biflexa serovar Patoc (strain Patoc 1 / ATCC 23582 / Paris) OX=456481 GN=motB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>sp|O07887|MOTB_TREPA Motility protein B OS=Treponema pallidum (strain Nichols) OX=243276 GN=motB PE=3 SV=1</t>
+  </si>
+  <si>
+    <t>tr|Q9K7W9|Q9K7W9_BACHD BH3239 protein OS=Bacillus halodurans (strain ATCC BAA-125 / DSM 18197 / FERM 7344 / JCM 9153 / C-125) OX=272558 GN=BH3239 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>KLU77742.1 flagellar motor protein MotB [Aliivibrio fischeri]</t>
+  </si>
+  <si>
+    <t>sp|O67122|MOTA_AQUAE Motility protein A OS=Aquifex aeolicus (strain VF5) OX=224324 GN=motA PE=3 SV=1</t>
+  </si>
+  <si>
+    <t>KPL93867.1 flagellar motor protein MotB [Vibrio splendidus]</t>
+  </si>
+  <si>
+    <t>tr|G3XD90|G3XD90_PSEAE MotD OS=Pseudomonas aeruginosa (strain ATCC 15692 / DSM 22644 / CIP 104116 / JCM 14847 / LMG 12228 / 1C / PRS 101 / PAO1) OX=208964 GN=motD PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|A0A1Q9FXY5|A0A1Q9FXY5_BACLI Flagellar motor protein MotS OS=Bacillus licheniformis OX=1402 GN=BHT94_18100 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|D3FX74|D3FX74_BACPE Flagellar motor rotation protein motS OS=Bacillus pseudofirmus (strain OF4) OX=398511 GN=motS PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>BAI86479.1 flagellar motor protein MotS [Bacillus subtilis subsp. natto BEST195]</t>
+  </si>
+  <si>
+    <t>tr|D4G048|D4G048_BACNB Flagellar motor protein MotS OS=Bacillus subtilis subsp. natto (strain BEST195) OX=645657 GN=motS PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|A0A2P1WLE1|A0A2P1WLE1_9BACI Flagellar motor protein MotS OS=Oceanobacillus iheyensis OX=182710 GN=OBCHQ24_11760 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|C0JPS8|C0JPS8_AERHY PomB2 OS=Aeromonas hydrophila OX=644 GN=pomB2 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|Q2N2L4|Q2N2L4_AERHY PomB OS=Aeromonas hydrophila OX=644 GN=pomB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|Q72ED9|Q72ED9_DESVH Chemotaxis protein PomB OS=Desulfovibrio vulgaris (strain Hildenborough / ATCC 29579 / DSM 644 / NCIMB 8303) OX=882 GN=pomB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>NP_717146.1 stator-force generator of Na+ coupled flagellar motor PomB [Shewanella oneidensis MR-1]</t>
+  </si>
+  <si>
+    <t>tr|O06874|O06874_VIBAL PomB OS=Vibrio alginolyticus OX=663 GN=pomB PE=1 SV=1</t>
+  </si>
+  <si>
+    <t>tr|Q9KTK9|Q9KTK9_VIBCH Chemotaxis protein PomB OS=Vibrio cholerae serotype O1 (strain ATCC 39315 / El Tor Inaba N16961) OX=243277 GN=VC_0893 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>WP_015296333.1 Polar Na+-driven flagellar motor protein MotB (PomB) [Vibrio parahaemolyticus]</t>
+  </si>
+  <si>
+    <t>tr|G9I2I5|G9I2I5_BACAO Flagellar motor protein OS=Bacillus alcalophilus OX=1445 GN=motS PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|A0A069DTH2|A0A069DTH2_9BACL Flagellar motor protein MotB OS=Paenibacillus sp. TCA20 OX=1499968 GN=TCA2_5830 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|A0A069DG39|A0A069DG39_9BACL Flagellar motor protein MotB OS=Paenibacillus sp. TCA20 OX=1499968 GN=TCA2_3718 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|Q72ZM9|Q72ZM9_BACC1 Sodium-driven polar flagellar protein PomB, putative OS=Bacillus cereus (strain ATCC 10987 / NRS 248) OX=222523 GN=BCE_4639 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>(H+ probably)</t>
+  </si>
+  <si>
+    <t>NP_719811.1 stator-force generator of H+ coupled flagellar motor MotB [Shewanella oneidensis MR-1]</t>
+  </si>
+  <si>
+    <t>Paenibacillus sp TCA20</t>
+  </si>
+  <si>
+    <t>tr|Q3BNW7|Q3BNW7_XANC5 Flagellar motor protein MotB OS=Xanthomonas campestris pv. vesicatoria (strain 85-10) OX=316273 GN=motB2 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>RpoN2- and FliA-regulated fliTX is indispensible for flagellar motility and virulence in Xanthomonas oryzae pv. Oryzae https://bmcmicrobiol.biomedcentral.com/articles/10.1186/s12866-017-1083-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terehara_etal_2009_PLoS1_Bacillus_Na_H_switch https://journals.plos.org/plosone/article?id=10.1371/journal.pone.0046248#s5 </t>
+  </si>
+  <si>
+    <t>Done:</t>
+  </si>
+  <si>
+    <t>Doesn't identify power source: https://www.nature.com/articles/s41598-018-24254-w</t>
+  </si>
+  <si>
+    <t>tr|Q3BU71|Q3BU71_XANC5 Flagellar motor protein MotB OS=Xanthomonas campestris pv. vesicatoria (strain 85-10) OX=316273 GN=motB1 PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|C4XNT9|C4XNT9_DESMR Chemotaxis protein MotB OS=Desulfovibrio magneticus (strain ATCC 700980 / DSM 13731 / RS-1) OX=573370 GN=motB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>tr|C4XNW2|C4XNW2_DESMR Chemotaxis protein MotB OS=Desulfovibrio magneticus (strain ATCC 700980 / DSM 13731 / RS-1) OX=573370 GN=motB PE=4 SV=1</t>
+  </si>
+  <si>
+    <t>Induction of the lateral flagellar system of Vibrio shilonii is an early event after inhibition of the sodium ion flux in the polar flagellum https://www.nrcresearchpress.com/doi/10.1139/cjm-2014-0579#.XbkUYanLfYU</t>
+  </si>
+  <si>
+    <t>Baccillus megaterium</t>
+  </si>
+  <si>
+    <t>AAU40425.3</t>
+  </si>
+  <si>
+    <t>ATP10434.1</t>
+  </si>
+  <si>
+    <t>ATP10768.1</t>
+  </si>
+  <si>
+    <t>Entero|Gamma_FB21|_|ATP10768.1|PomA [Aeromonas salmonicida subsp. pectinolytica 34mel]</t>
+  </si>
+  <si>
+    <t>Na+ (probably)</t>
+  </si>
+  <si>
+    <t>gb_name</t>
+  </si>
+  <si>
+    <t>QCG49373.1 flagellar motor stator protein MotA [Aeromonas schubertii]</t>
+  </si>
+  <si>
+    <t>QCG49373.1</t>
+  </si>
+  <si>
+    <t>ATP10434.1 flagellar motor protein MotA [Aeromonas salmonicida subsp. pectinolytica 34mel]</t>
+  </si>
+  <si>
+    <t>AAU40425.3 motility protein A flagellar stator MotA [Bacillus licheniformis DSM 13 = ATCC 14580]</t>
+  </si>
+  <si>
+    <t>CAB13242.1</t>
+  </si>
+  <si>
+    <t>BAH74235.1</t>
+  </si>
+  <si>
+    <t>BAH74235.1 chemotaxis protein MotA [Solidesulfovibrio magneticus RS-1]
+BAH75058.1 chemotaxis protein MotA [Solidesulfovibrio magneticus RS-1]</t>
+  </si>
+  <si>
+    <t>CAB14951.1 sodium channel stator-force generator subunit of flagellar rotation [Bacillus subtilis subsp. subtilis str. 168]</t>
+  </si>
+  <si>
+    <t>CAB14951.1</t>
+  </si>
+  <si>
+    <t>AAC74960.1 motility protein A [Escherichia coli str. K-12 substr. MG1655]</t>
+  </si>
+  <si>
+    <t>AAC74960.1</t>
+  </si>
+  <si>
+    <t>BAD76815.1 motility protein A (flagellar motor rotation) [Geobacillus kaustophilus HTA426]</t>
+  </si>
+  <si>
+    <t>AFV42026.1 flagellar motor protein MotA [Helicobacter pylori 26695]</t>
+  </si>
+  <si>
+    <t>BAC14501.1 motility protein A (flagellar motor rotation) [Oceanobacillus iheyensis HTE831]</t>
+  </si>
+  <si>
+    <t>BAC14181.1 flagellar motor aparatus [Oceanobacillus iheyensis HTE831]</t>
+  </si>
+  <si>
+    <t>AOP60447.1 flagellar motor stator protein MotA [Pseudomonas aeruginosa]
+AOP58989.1 flagellar motor protein [Pseudomonas aeruginosa]
+AAG04849.1 MotC [Pseudomonas aeruginosa PAO1]</t>
+  </si>
+  <si>
+    <t>WP_002721884.1 flagellar motor stator protein MotA [Cereibacter sphaeroides]</t>
+  </si>
+  <si>
+    <t>AAL20839.1 proton conductor component of motor [Salmonella enterica subsp. enterica serovar Typhimurium str. LT2]</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>AAD35759.1 motility protein A [Thermotoga maritima MSB8]</t>
+  </si>
+  <si>
+    <t>EDR32241.1 chemotaxis protein motA [Yersinia pestis biovar Orientalis str. IP275]</t>
+  </si>
+  <si>
+    <t>ACM24086.1 Motility protein A [Thermotoga neapolitana DSM 4359]</t>
+  </si>
+  <si>
+    <t>BAD64518.1 motility protein A [Alkalihalobacillus clausii KSM-K16]</t>
+  </si>
+  <si>
+    <t>ABZ98915.1 Chemotaxis MotA protein; putative membrane protein; putative signal peptide [Leptospira biflexa serovar Patoc strain 'Patoc 1 (Paris)']</t>
+  </si>
+  <si>
+    <t>UOY13875.1 motility protein A [Treponema pallidum subsp. pallidum]
+AWG41586.1 Mot family proton (H+) or sodium (Na+) transporter MotA [Treponema pallidum subsp. pertenue]</t>
+  </si>
+  <si>
+    <t>BAB06959.1 flagellar motor apparatus [Halalkalibacterium halodurans C-125]</t>
+  </si>
+  <si>
+    <t>AAW85209.1 flagellar motor protein MotA1 [Aliivibrio fischeri ES114]
+AAW87256.1 flagellar motor protein MotA2 [Aliivibrio fischeri ES114]</t>
+  </si>
+  <si>
+    <t>AAC07083.1 flagellar motor protein MotA [Aquifex aeolicus VF5]</t>
+  </si>
+  <si>
+    <t>EAP91937.1 flagellar motor protein [Vibrio splendidus 12B01]</t>
+  </si>
+  <si>
+    <t>AAG04849.1 MotC [Pseudomonas aeruginosa PAO1]
+AOP58989.1 flagellar motor protein [Pseudomonas aeruginosa]'</t>
+  </si>
+  <si>
+    <t>AAU41985.1 Na+-coupled flagellar stator MotP [Bacillus licheniformis DSM 13 = ATCC 14580]</t>
+  </si>
+  <si>
+    <t>ADC48830.1 Flagellar motor rotation protein motP [Alkalihalophilus pseudofirmus OF4]</t>
+  </si>
+  <si>
+    <t>CAB13242.1 motility protein A; MotA component of the H+-coupled stator flagellum complex [Bacillus subtilis subsp. subtilis str. 168]
+UUH67684.1 flagellar motor stator protein MotA [Bacillus subtilis subsp. natto]
+BAI84979.1 flagellar motor protein MotA [Bacillus subtilis subsp. natto BEST195]</t>
+  </si>
+  <si>
+    <t>BAI86480.1 flagellar motor protein MotP [Bacillus subtilis subsp. natto BEST195]
+BAI86480.1 flagellar motor protein MotP [Bacillus subtilis subsp. natto BEST195]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4736,6 +5036,13 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4766,10 +5073,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -4790,11 +5098,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5013,8 +5326,8 @@
   </sheetPr>
   <dimension ref="A1:AB344"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:I30"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="K85" sqref="A15:K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15985,10 +16298,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF3966B-1EAB-1C47-9D08-2620A952D7BC}">
-  <dimension ref="A1:Q949"/>
+  <dimension ref="A1:AB949"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15996,9 +16309,11 @@
     <col min="1" max="1" width="10.83203125" style="12"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="13" max="13" width="76.83203125" customWidth="1"/>
+    <col min="14" max="14" width="141.33203125" style="12" customWidth="1"/>
+    <col min="16" max="16" width="34.1640625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>1542</v>
       </c>
@@ -16023,10 +16338,49 @@
         <v>1541</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>1549</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>1548</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>1609</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>1535</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A2" s="12">
         <v>181</v>
       </c>
@@ -16057,14 +16411,42 @@
       <c r="L2" s="12">
         <v>339</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="7" t="s">
         <v>924</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="7" t="s">
+        <v>1550</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>1604</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>1613</v>
+      </c>
+      <c r="Q2" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" s="6"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A3" s="12">
         <v>530</v>
       </c>
@@ -16095,14 +16477,40 @@
       <c r="L3" s="12">
         <v>454</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="7" t="s">
         <v>1039</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="7" t="s">
+        <v>1551</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1605</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>1612</v>
+      </c>
+      <c r="Q3" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="6"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z3" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A4" s="12">
         <v>381</v>
       </c>
@@ -16115,14 +16523,40 @@
       <c r="L4" s="12">
         <v>679</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="7" t="s">
         <v>1264</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="7" t="s">
+        <v>1553</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>1611</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>1610</v>
+      </c>
+      <c r="Q4" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="6"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="112" x14ac:dyDescent="0.15">
       <c r="A5" s="12">
         <v>414</v>
       </c>
@@ -16135,14 +16569,42 @@
       <c r="L5" s="12">
         <v>340</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="7" t="s">
         <v>925</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="7" t="s">
+        <v>1552</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1614</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>1642</v>
+      </c>
+      <c r="Q5" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y5" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z5" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="49" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>562</v>
       </c>
@@ -16155,14 +16617,42 @@
       <c r="L6" s="12">
         <v>458</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="7" t="s">
         <v>1043</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="7" t="s">
+        <v>1554</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>1615</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>1616</v>
+      </c>
+      <c r="Q6" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S6" s="6"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y6" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z6" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>511</v>
       </c>
@@ -16178,11 +16668,39 @@
       <c r="M7" s="12" t="s">
         <v>746</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="N7" s="7" t="s">
+        <v>1555</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>1620</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>1619</v>
+      </c>
+      <c r="Q7" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S7" s="6"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>268</v>
       </c>
@@ -16195,14 +16713,39 @@
       <c r="L8" s="12">
         <v>343</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="M8" s="7" t="s">
         <v>928</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="N8" s="7" t="s">
+        <v>1556</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>1621</v>
+      </c>
+      <c r="Q8" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S8" s="6"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z8" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A9" s="12">
         <v>271</v>
       </c>
@@ -16215,14 +16758,41 @@
       <c r="L9" s="12">
         <v>104</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="M9" s="7" t="s">
         <v>689</v>
       </c>
-      <c r="N9" s="12" t="s">
+      <c r="N9" s="7" t="s">
+        <v>1557</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>1622</v>
+      </c>
+      <c r="Q9" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="6"/>
+      <c r="T9" s="3">
+        <v>210</v>
+      </c>
+      <c r="U9" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y9" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z9" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A10" s="12">
         <v>267</v>
       </c>
@@ -16235,14 +16805,39 @@
       <c r="L10" s="12">
         <v>328</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="7" t="s">
         <v>913</v>
       </c>
-      <c r="N10" s="12" t="s">
+      <c r="N10" s="7" t="s">
+        <v>1558</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>1623</v>
+      </c>
+      <c r="Q10" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S10" s="6"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y10" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z10" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A11" s="12">
         <v>266</v>
       </c>
@@ -16253,16 +16848,40 @@
         <v>3</v>
       </c>
       <c r="L11" s="12">
-        <v>164</v>
+        <v>328</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>749</v>
+        <v>913</v>
       </c>
       <c r="N11" s="12" t="s">
+        <v>1558</v>
+      </c>
+      <c r="P11" s="12" t="s">
+        <v>1623</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" s="6"/>
+      <c r="T11" s="3">
+        <v>182710</v>
+      </c>
+      <c r="U11" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="Y11" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z11" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="84" x14ac:dyDescent="0.15">
       <c r="A12" s="12">
         <v>289</v>
       </c>
@@ -16273,16 +16892,41 @@
         <v>3</v>
       </c>
       <c r="L12" s="12">
-        <v>103</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>688</v>
-      </c>
-      <c r="N12" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>1559</v>
+      </c>
+      <c r="P12" s="17" t="s">
+        <v>1625</v>
+      </c>
+      <c r="Q12" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S12" s="6"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y12" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z12" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A13" s="12">
         <v>675</v>
       </c>
@@ -16293,16 +16937,41 @@
         <v>3</v>
       </c>
       <c r="L13" s="12">
-        <v>162</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>747</v>
-      </c>
-      <c r="N13" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>688</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>1560</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>1626</v>
+      </c>
+      <c r="Q13" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S13" s="6"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y13" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z13" s="12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A14" s="12">
         <v>453</v>
       </c>
@@ -16313,16 +16982,41 @@
         <v>3</v>
       </c>
       <c r="L14" s="12">
-        <v>330</v>
+        <v>162</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>915</v>
+        <v>747</v>
       </c>
       <c r="N14" s="12" t="s">
+        <v>1561</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>1627</v>
+      </c>
+      <c r="Q14" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S14" s="6"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z14" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A15" s="12">
         <v>356</v>
       </c>
@@ -16333,16 +17027,39 @@
         <v>3</v>
       </c>
       <c r="L15" s="12">
-        <v>341</v>
-      </c>
-      <c r="M15" s="12" t="s">
-        <v>926</v>
-      </c>
-      <c r="N15" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>915</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>1562</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>1628</v>
+      </c>
+      <c r="Q15" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S15" s="6"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="Z15" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A16" s="12">
         <v>649</v>
       </c>
@@ -16353,16 +17070,39 @@
         <v>3</v>
       </c>
       <c r="L16" s="12">
-        <v>154</v>
-      </c>
-      <c r="M16" s="12" t="s">
-        <v>739</v>
+        <v>341</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>926</v>
       </c>
       <c r="N16" s="12" t="s">
+        <v>1563</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>1628</v>
+      </c>
+      <c r="Q16" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S16" s="6"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="Z16" s="12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A17" s="12">
         <v>538</v>
       </c>
@@ -16373,16 +17113,43 @@
         <v>3</v>
       </c>
       <c r="L17" s="12">
-        <v>160</v>
-      </c>
-      <c r="M17" s="12" t="s">
-        <v>745</v>
-      </c>
-      <c r="N17" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>739</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>1564</v>
+      </c>
+      <c r="P17" s="12" t="s">
+        <v>1629</v>
+      </c>
+      <c r="Q17" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S17" s="6"/>
+      <c r="T17" s="3">
+        <v>2336</v>
+      </c>
+      <c r="U17" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y17" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z17" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A18" s="12">
         <v>565</v>
       </c>
@@ -16393,16 +17160,41 @@
         <v>3</v>
       </c>
       <c r="L18" s="12">
-        <v>155</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>740</v>
+        <v>160</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>745</v>
       </c>
       <c r="N18" s="12" t="s">
+        <v>1565</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>1630</v>
+      </c>
+      <c r="Q18" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S18" s="6"/>
+      <c r="T18" s="3">
+        <v>632</v>
+      </c>
+      <c r="U18" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="Z18" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A19" s="12">
         <v>540</v>
       </c>
@@ -16413,16 +17205,41 @@
         <v>3</v>
       </c>
       <c r="L19" s="12">
-        <v>296</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>881</v>
+        <v>155</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>740</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>1543</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
+        <v>1566</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>1631</v>
+      </c>
+      <c r="Q19" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S19" s="6"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y19" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z19" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A20" s="12">
         <v>183</v>
       </c>
@@ -16433,16 +17250,41 @@
         <v>4</v>
       </c>
       <c r="L20" s="12">
-        <v>156</v>
-      </c>
-      <c r="M20" s="12" t="s">
-        <v>741</v>
-      </c>
-      <c r="N20" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>1567</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>1632</v>
+      </c>
+      <c r="Q20" s="7" t="s">
         <v>1543</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S20" s="6"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y20" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="Z20" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="56" x14ac:dyDescent="0.15">
       <c r="A21" s="12">
         <v>303</v>
       </c>
@@ -16453,16 +17295,39 @@
         <v>5</v>
       </c>
       <c r="L21" s="12">
-        <v>450</v>
-      </c>
-      <c r="M21" s="12" t="s">
-        <v>1035</v>
-      </c>
-      <c r="N21" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="N21" s="12" t="s">
+        <v>1568</v>
+      </c>
+      <c r="P21" s="17" t="s">
+        <v>1633</v>
+      </c>
+      <c r="Q21" s="7" t="s">
         <v>1543</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S21" s="6"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6"/>
+      <c r="X21" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="70" x14ac:dyDescent="0.15">
       <c r="A22" s="12">
         <v>245</v>
       </c>
@@ -16473,16 +17338,43 @@
         <v>132</v>
       </c>
       <c r="L22" s="12">
-        <v>181</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>766</v>
+        <v>450</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>1035</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
+        <v>1569</v>
+      </c>
+      <c r="P22" s="17" t="s">
+        <v>1634</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>1543</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S22" s="6"/>
+      <c r="T22" s="3">
+        <v>160</v>
+      </c>
+      <c r="U22" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+      <c r="X22" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="Y22" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z22" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A23" s="12">
         <v>403</v>
       </c>
@@ -16493,16 +17385,41 @@
         <v>132</v>
       </c>
       <c r="L23" s="12">
-        <v>530</v>
-      </c>
-      <c r="M23" s="12" t="s">
-        <v>1115</v>
+        <v>181</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>766</v>
       </c>
       <c r="N23" s="7" t="s">
+        <v>1570</v>
+      </c>
+      <c r="P23" s="12" t="s">
+        <v>1635</v>
+      </c>
+      <c r="Q23" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S23" s="6"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+      <c r="X23" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y23" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z23" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="56" x14ac:dyDescent="0.15">
       <c r="A24" s="12">
         <v>510</v>
       </c>
@@ -16513,16 +17430,41 @@
         <v>132</v>
       </c>
       <c r="L24" s="12">
-        <v>381</v>
-      </c>
-      <c r="M24" s="12" t="s">
-        <v>966</v>
+        <v>530</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>1115</v>
       </c>
       <c r="N24" s="7" t="s">
+        <v>1571</v>
+      </c>
+      <c r="P24" s="17" t="s">
+        <v>1636</v>
+      </c>
+      <c r="Q24" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S24" s="6"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+      <c r="X24" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y24" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z24" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A25" s="12">
         <v>124</v>
       </c>
@@ -16533,16 +17475,39 @@
         <v>132</v>
       </c>
       <c r="L25" s="12">
-        <v>414</v>
-      </c>
-      <c r="M25" s="12" t="s">
-        <v>999</v>
+        <v>381</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>966</v>
       </c>
       <c r="N25" s="7" t="s">
+        <v>1572</v>
+      </c>
+      <c r="P25" s="17" t="s">
+        <v>1637</v>
+      </c>
+      <c r="Q25" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S25" s="6"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A26" s="12">
         <v>476</v>
       </c>
@@ -16553,16 +17518,22 @@
         <v>132</v>
       </c>
       <c r="L26" s="12">
-        <v>562</v>
+        <v>414</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>1147</v>
-      </c>
-      <c r="N26" s="7" t="s">
+        <v>999</v>
+      </c>
+      <c r="N26" s="12" t="s">
+        <v>1572</v>
+      </c>
+      <c r="P26" s="12" t="s">
+        <v>1637</v>
+      </c>
+      <c r="Q26" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:26" ht="28" x14ac:dyDescent="0.15">
       <c r="A27" s="12">
         <v>766</v>
       </c>
@@ -16573,16 +17544,41 @@
         <v>132</v>
       </c>
       <c r="L27" s="12">
-        <v>511</v>
-      </c>
-      <c r="M27" s="12" t="s">
-        <v>1096</v>
+        <v>562</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>1147</v>
       </c>
       <c r="N27" s="7" t="s">
+        <v>1573</v>
+      </c>
+      <c r="P27" s="17" t="s">
+        <v>1638</v>
+      </c>
+      <c r="Q27" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S27" s="6"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y27" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z27" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="56" x14ac:dyDescent="0.15">
       <c r="A28" s="12">
         <v>926</v>
       </c>
@@ -16593,16 +17589,41 @@
         <v>132</v>
       </c>
       <c r="L28" s="12">
-        <v>268</v>
-      </c>
-      <c r="M28" s="12" t="s">
-        <v>853</v>
+        <v>511</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>1096</v>
       </c>
       <c r="N28" s="7" t="s">
+        <v>1574</v>
+      </c>
+      <c r="P28" s="17" t="s">
+        <v>1639</v>
+      </c>
+      <c r="Q28" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R28" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S28" s="6"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y28" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="Z28" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="42" x14ac:dyDescent="0.15">
       <c r="A29" s="12">
         <v>106</v>
       </c>
@@ -16613,16 +17634,41 @@
         <v>132</v>
       </c>
       <c r="L29" s="12">
-        <v>271</v>
-      </c>
-      <c r="M29" s="12" t="s">
-        <v>856</v>
+        <v>268</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>853</v>
       </c>
       <c r="N29" s="7" t="s">
+        <v>1575</v>
+      </c>
+      <c r="P29" s="17" t="s">
+        <v>1640</v>
+      </c>
+      <c r="Q29" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S29" s="6"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y29" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z29" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="42" x14ac:dyDescent="0.15">
       <c r="A30" s="12">
         <v>358</v>
       </c>
@@ -16633,16 +17679,41 @@
         <v>132</v>
       </c>
       <c r="L30" s="12">
-        <v>267</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>852</v>
+        <v>271</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>856</v>
       </c>
       <c r="N30" s="7" t="s">
+        <v>1576</v>
+      </c>
+      <c r="P30" s="17" t="s">
+        <v>1641</v>
+      </c>
+      <c r="Q30" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R30" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S30" s="6"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="7" t="s">
+        <v>1547</v>
+      </c>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y30" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z30" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="12">
         <v>182</v>
       </c>
@@ -16653,16 +17724,44 @@
         <v>132</v>
       </c>
       <c r="L31" s="12">
-        <v>266</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>851</v>
-      </c>
-      <c r="N31" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>852</v>
+      </c>
+      <c r="N31" s="17" t="s">
+        <v>1577</v>
+      </c>
+      <c r="O31" t="s">
+        <v>1618</v>
+      </c>
+      <c r="P31" s="7" t="s">
+        <v>1617</v>
+      </c>
+      <c r="Q31" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="R31" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S31" s="6"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y31" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z31" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="56" x14ac:dyDescent="0.15">
       <c r="A32" s="12">
         <v>270</v>
       </c>
@@ -16673,16 +17772,41 @@
         <v>132</v>
       </c>
       <c r="L32" s="12">
-        <v>289</v>
-      </c>
-      <c r="M32" s="12" t="s">
-        <v>874</v>
+        <v>266</v>
+      </c>
+      <c r="M32" s="7" t="s">
+        <v>851</v>
       </c>
       <c r="N32" s="7" t="s">
+        <v>1578</v>
+      </c>
+      <c r="P32" s="17" t="s">
+        <v>1643</v>
+      </c>
+      <c r="Q32" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S32" s="6"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
+      <c r="X32" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y32" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z32" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A33" s="12">
         <v>175</v>
       </c>
@@ -16693,16 +17817,43 @@
         <v>132</v>
       </c>
       <c r="L33" s="12">
-        <v>675</v>
-      </c>
-      <c r="M33" s="12" t="s">
-        <v>1260</v>
-      </c>
-      <c r="N33" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>874</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>1579</v>
+      </c>
+      <c r="P33" s="7" t="s">
+        <v>1624</v>
+      </c>
+      <c r="Q33" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S33" s="6"/>
+      <c r="T33" s="3">
+        <v>182710</v>
+      </c>
+      <c r="U33" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="V33" s="6"/>
+      <c r="W33" s="6"/>
+      <c r="X33" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y33" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z33" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A34" s="12">
         <v>818</v>
       </c>
@@ -16713,16 +17864,39 @@
         <v>132</v>
       </c>
       <c r="L34" s="12">
-        <v>453</v>
-      </c>
-      <c r="M34" s="12" t="s">
-        <v>1038</v>
-      </c>
-      <c r="N34" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="M34" s="7" t="s">
+        <v>1260</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>1580</v>
+      </c>
+      <c r="Q34" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S34" s="6"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+      <c r="X34" s="12"/>
+      <c r="Y34" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z34" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA34" s="9" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A35" s="12">
         <v>108</v>
       </c>
@@ -16733,16 +17907,36 @@
         <v>132</v>
       </c>
       <c r="L35" s="12">
-        <v>356</v>
-      </c>
-      <c r="M35" s="12" t="s">
-        <v>941</v>
-      </c>
-      <c r="N35" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>1038</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>1581</v>
+      </c>
+      <c r="Q35" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R35" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S35" s="6"/>
+      <c r="T35" s="12"/>
+      <c r="U35" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="V35" s="6"/>
+      <c r="W35" s="6"/>
+      <c r="X35" s="12"/>
+      <c r="Y35" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z35" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A36" s="12">
         <v>139</v>
       </c>
@@ -16753,16 +17947,38 @@
         <v>132</v>
       </c>
       <c r="L36" s="12">
-        <v>649</v>
-      </c>
-      <c r="M36" s="12" t="s">
-        <v>1234</v>
-      </c>
-      <c r="N36" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="M36" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>1582</v>
+      </c>
+      <c r="Q36" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R36" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S36" s="6"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="V36" s="6"/>
+      <c r="W36" s="6"/>
+      <c r="X36" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y36" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z36" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A37" s="12">
         <v>83</v>
       </c>
@@ -16773,16 +17989,35 @@
         <v>132</v>
       </c>
       <c r="L37" s="12">
-        <v>538</v>
-      </c>
-      <c r="M37" s="12" t="s">
-        <v>1123</v>
-      </c>
-      <c r="N37" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>1234</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>1583</v>
+      </c>
+      <c r="Q37" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S37" s="6"/>
+      <c r="T37" s="12"/>
+      <c r="U37" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="V37" s="6"/>
+      <c r="W37" s="6"/>
+      <c r="X37" s="12"/>
+      <c r="Y37" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z37" s="12"/>
+      <c r="AA37" s="6"/>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A38" s="12">
         <v>84</v>
       </c>
@@ -16793,16 +18028,38 @@
         <v>132</v>
       </c>
       <c r="L38" s="12">
-        <v>565</v>
-      </c>
-      <c r="M38" s="12" t="s">
-        <v>1150</v>
-      </c>
-      <c r="N38" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="M38" s="7" t="s">
+        <v>1123</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>1584</v>
+      </c>
+      <c r="Q38" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R38" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S38" s="6"/>
+      <c r="T38" s="12"/>
+      <c r="U38" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="V38" s="6"/>
+      <c r="W38" s="6"/>
+      <c r="X38" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y38" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z38" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A39" s="12">
         <v>447</v>
       </c>
@@ -16813,16 +18070,38 @@
         <v>132</v>
       </c>
       <c r="L39" s="12">
-        <v>540</v>
-      </c>
-      <c r="M39" s="12" t="s">
-        <v>1125</v>
-      </c>
-      <c r="N39" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>1150</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>1585</v>
+      </c>
+      <c r="Q39" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R39" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S39" s="6"/>
+      <c r="T39" s="3">
+        <v>666</v>
+      </c>
+      <c r="U39" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="V39" s="6"/>
+      <c r="W39" s="6"/>
+      <c r="X39" s="12"/>
+      <c r="Y39" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z39" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A40" s="12">
         <v>449</v>
       </c>
@@ -16833,16 +18112,40 @@
         <v>132</v>
       </c>
       <c r="L40" s="12">
-        <v>183</v>
-      </c>
-      <c r="M40" s="12" t="s">
-        <v>768</v>
-      </c>
-      <c r="N40" s="7" t="s">
-        <v>1539</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.15">
+        <v>540</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>1125</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>1586</v>
+      </c>
+      <c r="Q40" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="R40" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S40" s="6"/>
+      <c r="T40" s="3">
+        <v>670</v>
+      </c>
+      <c r="U40" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="V40" s="6"/>
+      <c r="W40" s="6"/>
+      <c r="X40" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y40" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z40" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A41" s="12">
         <v>448</v>
       </c>
@@ -16853,16 +18156,41 @@
         <v>132</v>
       </c>
       <c r="L41" s="12">
-        <v>303</v>
-      </c>
-      <c r="M41" s="12" t="s">
-        <v>888</v>
-      </c>
-      <c r="N41" s="7" t="s">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.15">
+        <v>183</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>768</v>
+      </c>
+      <c r="N41" s="12" t="s">
+        <v>1587</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>1539</v>
+      </c>
+      <c r="R41" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S41" s="6"/>
+      <c r="T41" s="12"/>
+      <c r="U41" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="V41" s="6"/>
+      <c r="W41" s="6"/>
+      <c r="X41" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y41" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z41" s="7" t="s">
+        <v>1596</v>
+      </c>
+      <c r="AA41" s="18" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A42" s="12">
         <v>123</v>
       </c>
@@ -16872,18 +18200,37 @@
       <c r="C42" t="s">
         <v>132</v>
       </c>
+      <c r="L42" s="12">
+        <v>303</v>
+      </c>
       <c r="M42" s="7" t="s">
-        <v>1546</v>
-      </c>
-      <c r="N42" s="7" t="s">
-        <v>584</v>
-      </c>
-      <c r="O42" s="7" t="s">
-        <v>585</v>
-      </c>
-      <c r="Q42" s="12"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.15">
+        <v>888</v>
+      </c>
+      <c r="N42" s="12" t="s">
+        <v>1588</v>
+      </c>
+      <c r="Q42" s="7" t="s">
+        <v>1540</v>
+      </c>
+      <c r="R42" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S42" s="6"/>
+      <c r="T42" s="12"/>
+      <c r="U42" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="V42" s="6"/>
+      <c r="W42" s="6"/>
+      <c r="X42" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y42" s="12"/>
+      <c r="Z42" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A43" s="12">
         <v>133</v>
       </c>
@@ -16893,8 +18240,25 @@
       <c r="C43" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="M43" t="s">
+        <v>1593</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>1589</v>
+      </c>
+      <c r="Q43" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="R43" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S43" s="6"/>
+      <c r="T43" s="12"/>
+      <c r="U43" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A44" s="12">
         <v>141</v>
       </c>
@@ -16904,8 +18268,28 @@
       <c r="C44" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N44" s="7" t="s">
+        <v>1599</v>
+      </c>
+      <c r="R44" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S44" s="6"/>
+      <c r="T44" s="12"/>
+      <c r="U44" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="V44" s="6"/>
+      <c r="W44" s="6"/>
+      <c r="X44" s="12"/>
+      <c r="Y44" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z44" s="12" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A45" s="12">
         <v>787</v>
       </c>
@@ -16915,8 +18299,19 @@
       <c r="C45" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N45" s="7" t="s">
+        <v>1594</v>
+      </c>
+      <c r="R45" s="5"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="3">
+        <v>340</v>
+      </c>
+      <c r="U45" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A46" s="12">
         <v>196</v>
       </c>
@@ -16926,11 +18321,11 @@
       <c r="C46" t="s">
         <v>132</v>
       </c>
-      <c r="L46" s="7" t="s">
-        <v>1544</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N46" s="7" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A47" s="12">
         <v>420</v>
       </c>
@@ -16940,8 +18335,11 @@
       <c r="C47" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="N47" s="7" t="s">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A48" s="12">
         <v>816</v>
       </c>
@@ -16951,11 +18349,37 @@
       <c r="C48" t="s">
         <v>132</v>
       </c>
-      <c r="L48" s="7" t="s">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="N48" s="7" t="s">
+        <v>1590</v>
+      </c>
+      <c r="Q48" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="R48" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S48" s="6"/>
+      <c r="T48" s="12"/>
+      <c r="U48" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="V48" s="6"/>
+      <c r="W48" s="6"/>
+      <c r="X48" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y48" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z48" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA48" s="9"/>
+      <c r="AB48" s="12" t="s">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A49" s="12">
         <v>360</v>
       </c>
@@ -16965,8 +18389,28 @@
       <c r="C49" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="N49" s="12" t="s">
+        <v>1592</v>
+      </c>
+      <c r="Q49" s="7" t="s">
+        <v>1591</v>
+      </c>
+      <c r="R49" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S49" s="6"/>
+      <c r="T49" s="12"/>
+      <c r="U49" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="V49" s="6"/>
+      <c r="W49" s="6"/>
+      <c r="X49" s="12"/>
+      <c r="Y49" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A50" s="12">
         <v>365</v>
       </c>
@@ -16976,8 +18420,36 @@
       <c r="C50" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="M50" s="7" t="s">
+        <v>1603</v>
+      </c>
+      <c r="P50" s="7" t="s">
+        <v>1628</v>
+      </c>
+      <c r="Q50" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="R50" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S50" s="6"/>
+      <c r="T50" s="12"/>
+      <c r="U50" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="V50" s="6"/>
+      <c r="W50" s="6"/>
+      <c r="X50" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y50" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z50" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A51" s="12">
         <v>417</v>
       </c>
@@ -16987,8 +18459,27 @@
       <c r="C51" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="M51" s="7" t="s">
+        <v>1546</v>
+      </c>
+      <c r="N51" s="7"/>
+      <c r="P51" s="7" t="s">
+        <v>1628</v>
+      </c>
+      <c r="Q51" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="V51" s="6"/>
+      <c r="W51" s="6"/>
+      <c r="X51" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="Y51" s="12"/>
+      <c r="Z51" s="7" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A52" s="12">
         <v>743</v>
       </c>
@@ -16998,8 +18489,28 @@
       <c r="C52" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="L52" s="7" t="s">
+        <v>1544</v>
+      </c>
+      <c r="P52" s="7" t="s">
+        <v>1628</v>
+      </c>
+      <c r="Q52" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="U52" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="V52" s="6"/>
+      <c r="W52" s="6"/>
+      <c r="X52" s="12"/>
+      <c r="Y52" s="12"/>
+      <c r="Z52" s="12"/>
+      <c r="AA52" s="9" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A53" s="12">
         <v>169</v>
       </c>
@@ -17009,8 +18520,26 @@
       <c r="C53" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="P53" s="7" t="s">
+        <v>1628</v>
+      </c>
+      <c r="Q53" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="U53" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="V53" s="6"/>
+      <c r="W53" s="6"/>
+      <c r="X53" s="12"/>
+      <c r="Y53" s="12"/>
+      <c r="Z53" s="12"/>
+      <c r="AA53" s="9" t="s">
+        <v>1602</v>
+      </c>
+      <c r="AB53" s="12"/>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A54" s="12">
         <v>385</v>
       </c>
@@ -17020,8 +18549,11 @@
       <c r="C54" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="L54" s="7" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A55" s="12">
         <v>798</v>
       </c>
@@ -17031,8 +18563,18 @@
       <c r="C55" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="N55" s="12" t="s">
+        <v>1607</v>
+      </c>
+      <c r="O55" s="7" t="s">
+        <v>1606</v>
+      </c>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7" t="s">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A56" s="12">
         <v>147</v>
       </c>
@@ -17043,7 +18585,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A57" s="12">
         <v>146</v>
       </c>
@@ -17054,7 +18596,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A58" s="12">
         <v>148</v>
       </c>
@@ -17065,7 +18607,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A59" s="12">
         <v>479</v>
       </c>
@@ -17076,7 +18618,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A60" s="12">
         <v>167</v>
       </c>
@@ -17087,7 +18629,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A61" s="12">
         <v>796</v>
       </c>
@@ -17098,7 +18640,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A62" s="12">
         <v>795</v>
       </c>
@@ -17109,7 +18651,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A63" s="12">
         <v>797</v>
       </c>
@@ -17120,7 +18662,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A64" s="12">
         <v>166</v>
       </c>
@@ -17130,8 +18672,12 @@
       <c r="C64" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA64" s="12"/>
+      <c r="AB64" s="9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A65" s="12">
         <v>12</v>
       </c>
@@ -17141,8 +18687,10 @@
       <c r="C65" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA65" s="6"/>
+      <c r="AB65" s="6"/>
+    </row>
+    <row r="66" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="12">
         <v>435</v>
       </c>
@@ -17152,8 +18700,29 @@
       <c r="C66" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R66" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S66" s="6"/>
+      <c r="T66" s="12"/>
+      <c r="U66" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="V66" s="6"/>
+      <c r="W66" s="6"/>
+      <c r="X66" s="12"/>
+      <c r="Y66" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z66" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA66" s="6"/>
+      <c r="AB66" s="13" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A67" s="12">
         <v>125</v>
       </c>
@@ -17163,8 +18732,21 @@
       <c r="C67" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R67" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S67" s="6"/>
+      <c r="T67" s="12"/>
+      <c r="U67" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="V67" s="6"/>
+      <c r="W67" s="6"/>
+      <c r="X67" s="12"/>
+      <c r="Y67" s="12"/>
+      <c r="Z67" s="12"/>
+    </row>
+    <row r="68" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A68" s="12">
         <v>390</v>
       </c>
@@ -17174,8 +18756,23 @@
       <c r="C68" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="V68" s="6"/>
+      <c r="W68" s="6"/>
+      <c r="X68" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y68" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z68" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA68" s="6"/>
+      <c r="AB68" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A69" s="12">
         <v>393</v>
       </c>
@@ -17185,8 +18782,23 @@
       <c r="C69" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R69" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="S69" s="6"/>
+      <c r="T69" s="12"/>
+      <c r="U69" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="V69" s="6"/>
+      <c r="W69" s="6"/>
+      <c r="X69" s="12"/>
+      <c r="Y69" s="12"/>
+      <c r="Z69" s="12"/>
+      <c r="AA69" s="6"/>
+      <c r="AB69" s="6"/>
+    </row>
+    <row r="70" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A70" s="12">
         <v>413</v>
       </c>
@@ -17196,8 +18808,10 @@
       <c r="C70" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA70" s="6"/>
+      <c r="AB70" s="6"/>
+    </row>
+    <row r="71" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A71" s="12">
         <v>412</v>
       </c>
@@ -17207,8 +18821,23 @@
       <c r="C71" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R71" s="5"/>
+      <c r="S71" s="6"/>
+      <c r="T71" s="3">
+        <v>83334</v>
+      </c>
+      <c r="U71" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="V71" s="6"/>
+      <c r="W71" s="6"/>
+      <c r="X71" s="12"/>
+      <c r="Y71" s="12"/>
+      <c r="Z71" s="12"/>
+      <c r="AA71" s="6"/>
+      <c r="AB71" s="6"/>
+    </row>
+    <row r="72" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A72" s="12">
         <v>853</v>
       </c>
@@ -17218,8 +18847,23 @@
       <c r="C72" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R72" s="5"/>
+      <c r="S72" s="6"/>
+      <c r="T72" s="3">
+        <v>155864</v>
+      </c>
+      <c r="U72" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="V72" s="6"/>
+      <c r="W72" s="6"/>
+      <c r="X72" s="12"/>
+      <c r="Y72" s="12"/>
+      <c r="Z72" s="12"/>
+      <c r="AA72" s="6"/>
+      <c r="AB72" s="6"/>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A73" s="12">
         <v>384</v>
       </c>
@@ -17229,8 +18873,23 @@
       <c r="C73" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R73" s="5"/>
+      <c r="S73" s="6"/>
+      <c r="T73" s="3">
+        <v>217992</v>
+      </c>
+      <c r="U73" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="V73" s="6"/>
+      <c r="W73" s="6"/>
+      <c r="X73" s="12"/>
+      <c r="Y73" s="12"/>
+      <c r="Z73" s="12"/>
+      <c r="AA73" s="6"/>
+      <c r="AB73" s="6"/>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A74" s="12">
         <v>788</v>
       </c>
@@ -17240,8 +18899,10 @@
       <c r="C74" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA74" s="6"/>
+      <c r="AB74" s="6"/>
+    </row>
+    <row r="75" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A75" s="12">
         <v>943</v>
       </c>
@@ -17251,8 +18912,23 @@
       <c r="C75" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R75" s="6"/>
+      <c r="S75" s="6"/>
+      <c r="T75" s="3">
+        <v>209261</v>
+      </c>
+      <c r="U75" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="V75" s="6"/>
+      <c r="W75" s="6"/>
+      <c r="X75" s="12"/>
+      <c r="Y75" s="12"/>
+      <c r="Z75" s="12"/>
+      <c r="AA75" s="6"/>
+      <c r="AB75" s="6"/>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A76" s="12">
         <v>942</v>
       </c>
@@ -17262,8 +18938,23 @@
       <c r="C76" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R76" s="6"/>
+      <c r="S76" s="6"/>
+      <c r="T76" s="3">
+        <v>601</v>
+      </c>
+      <c r="U76" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="V76" s="6"/>
+      <c r="W76" s="6"/>
+      <c r="X76" s="12"/>
+      <c r="Y76" s="12"/>
+      <c r="Z76" s="12"/>
+      <c r="AA76" s="6"/>
+      <c r="AB76" s="6"/>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A77" s="12">
         <v>262</v>
       </c>
@@ -17273,8 +18964,23 @@
       <c r="C77" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R77" s="6"/>
+      <c r="S77" s="6"/>
+      <c r="T77" s="3">
+        <v>602</v>
+      </c>
+      <c r="U77" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="V77" s="6"/>
+      <c r="W77" s="6"/>
+      <c r="X77" s="12"/>
+      <c r="Y77" s="12"/>
+      <c r="Z77" s="12"/>
+      <c r="AA77" s="6"/>
+      <c r="AB77" s="6"/>
+    </row>
+    <row r="78" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A78" s="12">
         <v>265</v>
       </c>
@@ -17284,8 +18990,10 @@
       <c r="C78" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA78" s="6"/>
+      <c r="AB78" s="6"/>
+    </row>
+    <row r="79" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A79" s="12">
         <v>264</v>
       </c>
@@ -17295,8 +19003,23 @@
       <c r="C79" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R79" s="5"/>
+      <c r="S79" s="6"/>
+      <c r="T79" s="3">
+        <v>198094</v>
+      </c>
+      <c r="U79" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="V79" s="6"/>
+      <c r="W79" s="6"/>
+      <c r="X79" s="12"/>
+      <c r="Y79" s="12"/>
+      <c r="Z79" s="12"/>
+      <c r="AA79" s="6"/>
+      <c r="AB79" s="6"/>
+    </row>
+    <row r="80" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A80" s="12">
         <v>919</v>
       </c>
@@ -17306,8 +19029,23 @@
       <c r="C80" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R80" s="5"/>
+      <c r="S80" s="6"/>
+      <c r="T80" s="3">
+        <v>222523</v>
+      </c>
+      <c r="U80" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="V80" s="6"/>
+      <c r="W80" s="6"/>
+      <c r="X80" s="12"/>
+      <c r="Y80" s="12"/>
+      <c r="Z80" s="12"/>
+      <c r="AA80" s="6"/>
+      <c r="AB80" s="6"/>
+    </row>
+    <row r="81" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A81" s="12">
         <v>891</v>
       </c>
@@ -17317,8 +19055,23 @@
       <c r="C81" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R81" s="5"/>
+      <c r="S81" s="6"/>
+      <c r="T81" s="3">
+        <v>226900</v>
+      </c>
+      <c r="U81" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="V81" s="6"/>
+      <c r="W81" s="6"/>
+      <c r="X81" s="12"/>
+      <c r="Y81" s="12"/>
+      <c r="Z81" s="12"/>
+      <c r="AA81" s="6"/>
+      <c r="AB81" s="6"/>
+    </row>
+    <row r="82" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A82" s="12">
         <v>379</v>
       </c>
@@ -17328,8 +19081,23 @@
       <c r="C82" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R82" s="5"/>
+      <c r="S82" s="6"/>
+      <c r="T82" s="3">
+        <v>86665</v>
+      </c>
+      <c r="U82" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="V82" s="6"/>
+      <c r="W82" s="6"/>
+      <c r="X82" s="12"/>
+      <c r="Y82" s="12"/>
+      <c r="Z82" s="12"/>
+      <c r="AA82" s="6"/>
+      <c r="AB82" s="6"/>
+    </row>
+    <row r="83" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A83" s="12">
         <v>380</v>
       </c>
@@ -17339,8 +19107,22 @@
       <c r="C83" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R83" s="5"/>
+      <c r="S83" s="6"/>
+      <c r="T83" s="3">
+        <v>1423</v>
+      </c>
+      <c r="U83" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="V83" s="6"/>
+      <c r="W83" s="6"/>
+      <c r="X83" s="12"/>
+      <c r="Y83" s="12"/>
+      <c r="Z83" s="12"/>
+      <c r="AB83" s="6"/>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A84" s="12">
         <v>259</v>
       </c>
@@ -17350,8 +19132,9 @@
       <c r="C84" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AB84" s="6"/>
+    </row>
+    <row r="85" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A85" s="12">
         <v>101</v>
       </c>
@@ -17361,8 +19144,9 @@
       <c r="C85" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AB85" s="6"/>
+    </row>
+    <row r="86" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A86" s="12">
         <v>58</v>
       </c>
@@ -17372,8 +19156,18 @@
       <c r="C86" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="U86" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="V86" s="6"/>
+      <c r="W86" s="6"/>
+      <c r="X86" s="12"/>
+      <c r="Y86" s="12"/>
+      <c r="Z86" s="12"/>
+      <c r="AA86" s="6"/>
+      <c r="AB86" s="6"/>
+    </row>
+    <row r="87" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A87" s="12">
         <v>95</v>
       </c>
@@ -17383,8 +19177,16 @@
       <c r="C87" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="T87" s="3">
+        <v>672</v>
+      </c>
+      <c r="U87" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA87" s="6"/>
+      <c r="AB87" s="6"/>
+    </row>
+    <row r="88" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A88" s="12">
         <v>669</v>
       </c>
@@ -17394,8 +19196,16 @@
       <c r="C88" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="T88" s="3">
+        <v>196600</v>
+      </c>
+      <c r="U88" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="AA88" s="6"/>
+      <c r="AB88" s="6"/>
+    </row>
+    <row r="89" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A89" s="12">
         <v>127</v>
       </c>
@@ -17405,8 +19215,13 @@
       <c r="C89" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="U89" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="AA89" s="6"/>
+      <c r="AB89" s="6"/>
+    </row>
+    <row r="90" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A90" s="12">
         <v>761</v>
       </c>
@@ -17416,8 +19231,23 @@
       <c r="C90" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R90" s="5"/>
+      <c r="S90" s="6"/>
+      <c r="T90" s="3">
+        <v>229193</v>
+      </c>
+      <c r="U90" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="V90" s="6"/>
+      <c r="W90" s="6"/>
+      <c r="X90" s="12"/>
+      <c r="Y90" s="12"/>
+      <c r="Z90" s="12"/>
+      <c r="AA90" s="6"/>
+      <c r="AB90" s="6"/>
+    </row>
+    <row r="91" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A91" s="12">
         <v>218</v>
       </c>
@@ -17427,8 +19257,23 @@
       <c r="C91" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R91" s="5"/>
+      <c r="S91" s="6"/>
+      <c r="T91" s="3">
+        <v>187410</v>
+      </c>
+      <c r="U91" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="V91" s="6"/>
+      <c r="W91" s="6"/>
+      <c r="X91" s="12"/>
+      <c r="Y91" s="12"/>
+      <c r="Z91" s="12"/>
+      <c r="AA91" s="6"/>
+      <c r="AB91" s="6"/>
+    </row>
+    <row r="92" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A92" s="12">
         <v>172</v>
       </c>
@@ -17438,8 +19283,10 @@
       <c r="C92" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA92" s="6"/>
+      <c r="AB92" s="6"/>
+    </row>
+    <row r="93" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A93" s="12">
         <v>203</v>
       </c>
@@ -17449,8 +19296,23 @@
       <c r="C93" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R93" s="5"/>
+      <c r="S93" s="6"/>
+      <c r="T93" s="3">
+        <v>92829</v>
+      </c>
+      <c r="U93" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="V93" s="6"/>
+      <c r="W93" s="6"/>
+      <c r="X93" s="12"/>
+      <c r="Y93" s="12"/>
+      <c r="Z93" s="12"/>
+      <c r="AA93" s="6"/>
+      <c r="AB93" s="6"/>
+    </row>
+    <row r="94" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A94" s="12">
         <v>415</v>
       </c>
@@ -17460,8 +19322,17 @@
       <c r="C94" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="V94" s="6"/>
+      <c r="W94" s="6"/>
+      <c r="X94" s="12"/>
+      <c r="Y94" s="12"/>
+      <c r="Z94" s="12"/>
+      <c r="AA94" s="9" t="s">
+        <v>1595</v>
+      </c>
+      <c r="AB94" s="6"/>
+    </row>
+    <row r="95" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A95" s="12">
         <v>346</v>
       </c>
@@ -17471,8 +19342,17 @@
       <c r="C95" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="T95" s="3">
+        <v>882</v>
+      </c>
+      <c r="U95" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="V95" s="6"/>
+      <c r="AA95" s="6"/>
+      <c r="AB95" s="6"/>
+    </row>
+    <row r="96" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A96" s="12">
         <v>345</v>
       </c>
@@ -17482,8 +19362,22 @@
       <c r="C96" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="R96" s="5"/>
+      <c r="S96" s="6"/>
+      <c r="T96" s="3">
+        <v>85963</v>
+      </c>
+      <c r="U96" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="W96" s="6"/>
+      <c r="X96" s="12"/>
+      <c r="Y96" s="12"/>
+      <c r="Z96" s="12"/>
+      <c r="AA96" s="6"/>
+      <c r="AB96" s="6"/>
+    </row>
+    <row r="97" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A97" s="12">
         <v>946</v>
       </c>
@@ -17493,8 +19387,10 @@
       <c r="C97" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA97" s="6"/>
+      <c r="AB97" s="6"/>
+    </row>
+    <row r="98" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A98" s="12">
         <v>389</v>
       </c>
@@ -17504,8 +19400,10 @@
       <c r="C98" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA98" s="6"/>
+      <c r="AB98" s="6"/>
+    </row>
+    <row r="99" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A99" s="12">
         <v>406</v>
       </c>
@@ -17515,8 +19413,13 @@
       <c r="C99" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="U99" s="7" t="s">
+        <v>1597</v>
+      </c>
+      <c r="AA99" s="6"/>
+      <c r="AB99" s="6"/>
+    </row>
+    <row r="100" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A100" s="12">
         <v>408</v>
       </c>
@@ -17526,8 +19429,19 @@
       <c r="C100" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="U100" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="V100" s="10"/>
+      <c r="W100" s="10"/>
+      <c r="X100" s="7"/>
+      <c r="Y100" s="7"/>
+      <c r="Z100" s="7"/>
+      <c r="AA100" s="18" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A101" s="12">
         <v>404</v>
       </c>
@@ -17537,8 +19451,20 @@
       <c r="C101" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="U101" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="V101" s="6"/>
+      <c r="W101" s="6"/>
+      <c r="X101" s="12"/>
+      <c r="Y101" s="12"/>
+      <c r="Z101" s="12"/>
+      <c r="AA101" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB101" s="6"/>
+    </row>
+    <row r="102" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A102" s="12">
         <v>57</v>
       </c>
@@ -17548,8 +19474,10 @@
       <c r="C102" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA102" s="6"/>
+      <c r="AB102" s="6"/>
+    </row>
+    <row r="103" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A103" s="12">
         <v>197</v>
       </c>
@@ -17559,8 +19487,10 @@
       <c r="C103" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA103" s="6"/>
+      <c r="AB103" s="6"/>
+    </row>
+    <row r="104" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A104" s="12">
         <v>377</v>
       </c>
@@ -17570,8 +19500,10 @@
       <c r="C104" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA104" s="6"/>
+      <c r="AB104" s="6"/>
+    </row>
+    <row r="105" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A105" s="12">
         <v>126</v>
       </c>
@@ -17581,8 +19513,10 @@
       <c r="C105" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA105" s="6"/>
+      <c r="AB105" s="6"/>
+    </row>
+    <row r="106" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A106" s="12">
         <v>854</v>
       </c>
@@ -17592,8 +19526,10 @@
       <c r="C106" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA106" s="6"/>
+      <c r="AB106" s="6"/>
+    </row>
+    <row r="107" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A107" s="12">
         <v>720</v>
       </c>
@@ -17603,8 +19539,10 @@
       <c r="C107" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA107" s="6"/>
+      <c r="AB107" s="6"/>
+    </row>
+    <row r="108" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A108" s="12">
         <v>845</v>
       </c>
@@ -17614,8 +19552,10 @@
       <c r="C108" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA108" s="6"/>
+      <c r="AB108" s="6"/>
+    </row>
+    <row r="109" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A109" s="12">
         <v>501</v>
       </c>
@@ -17625,8 +19565,10 @@
       <c r="C109" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA109" s="6"/>
+      <c r="AB109" s="6"/>
+    </row>
+    <row r="110" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A110" s="12">
         <v>709</v>
       </c>
@@ -17636,8 +19578,10 @@
       <c r="C110" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA110" s="6"/>
+      <c r="AB110" s="6"/>
+    </row>
+    <row r="111" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A111" s="12">
         <v>180</v>
       </c>
@@ -17647,8 +19591,10 @@
       <c r="C111" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA111" s="6"/>
+      <c r="AB111" s="6"/>
+    </row>
+    <row r="112" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A112" s="12">
         <v>240</v>
       </c>
@@ -17658,8 +19604,10 @@
       <c r="C112" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA112" s="6"/>
+      <c r="AB112" s="6"/>
+    </row>
+    <row r="113" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A113" s="12">
         <v>232</v>
       </c>
@@ -17669,8 +19617,10 @@
       <c r="C113" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA113" s="6"/>
+      <c r="AB113" s="6"/>
+    </row>
+    <row r="114" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A114" s="12">
         <v>714</v>
       </c>
@@ -17680,8 +19630,10 @@
       <c r="C114" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA114" s="6"/>
+      <c r="AB114" s="6"/>
+    </row>
+    <row r="115" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A115" s="12">
         <v>225</v>
       </c>
@@ -17691,8 +19643,10 @@
       <c r="C115" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA115" s="6"/>
+      <c r="AB115" s="6"/>
+    </row>
+    <row r="116" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A116" s="12">
         <v>248</v>
       </c>
@@ -17702,8 +19656,10 @@
       <c r="C116" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA116" s="6"/>
+      <c r="AB116" s="6"/>
+    </row>
+    <row r="117" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A117" s="12">
         <v>242</v>
       </c>
@@ -17713,8 +19669,10 @@
       <c r="C117" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA117" s="6"/>
+      <c r="AB117" s="6"/>
+    </row>
+    <row r="118" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A118" s="12">
         <v>231</v>
       </c>
@@ -17724,8 +19682,10 @@
       <c r="C118" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA118" s="6"/>
+      <c r="AB118" s="6"/>
+    </row>
+    <row r="119" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A119" s="12">
         <v>916</v>
       </c>
@@ -17735,8 +19695,10 @@
       <c r="C119" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA119" s="6"/>
+      <c r="AB119" s="6"/>
+    </row>
+    <row r="120" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A120" s="12">
         <v>915</v>
       </c>
@@ -17747,7 +19709,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A121" s="12">
         <v>912</v>
       </c>
@@ -17757,8 +19719,10 @@
       <c r="C121" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="AA121" s="6"/>
+      <c r="AB121" s="6"/>
+    </row>
+    <row r="122" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A122" s="12">
         <v>207</v>
       </c>
@@ -17769,7 +19733,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A123" s="12">
         <v>431</v>
       </c>
@@ -17780,7 +19744,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A124" s="12">
         <v>800</v>
       </c>
@@ -17791,7 +19755,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A125" s="12">
         <v>506</v>
       </c>
@@ -17802,7 +19766,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A126" s="12">
         <v>505</v>
       </c>
@@ -17813,7 +19777,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A127" s="12">
         <v>483</v>
       </c>
@@ -17824,7 +19788,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A128" s="12">
         <v>482</v>
       </c>
@@ -26871,6 +28835,17 @@
     <sortCondition ref="C2:C949"/>
     <sortCondition ref="B2:B949"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="AA52" r:id="rId1" location=".XbkUYanLfYU" display="https://www.nrcresearchpress.com/doi/10.1139/cjm-2014-0579#.XbkUYanLfYU" xr:uid="{471ABF49-BE4A-0242-A711-7803A87C6B64}"/>
+    <hyperlink ref="AA101" r:id="rId2" xr:uid="{0F232809-AE10-5C45-88D6-3490B3E0E81B}"/>
+    <hyperlink ref="AB68" r:id="rId3" xr:uid="{EB623F04-1C5B-1D42-896A-BDA83E4F32CA}"/>
+    <hyperlink ref="AA94" r:id="rId4" display="https://bmcmicrobiol.biomedcentral.com/articles/10.1186/s12866-017-1083-6" xr:uid="{6B34B929-442B-0F4B-A26C-22D642005A15}"/>
+    <hyperlink ref="AA34" r:id="rId5" xr:uid="{A4066CD0-4055-4843-B670-B7565041CA73}"/>
+    <hyperlink ref="AB64" r:id="rId6" xr:uid="{0497EF01-0FBE-E940-A9EC-7FB801AAF40D}"/>
+    <hyperlink ref="AA41" r:id="rId7" xr:uid="{3B0C2CB6-0B47-D042-9BD6-9B7D41472891}"/>
+    <hyperlink ref="AA100" r:id="rId8" xr:uid="{EE1CC525-EF01-F740-AAEE-DF970AE12F65}"/>
+    <hyperlink ref="AA53" r:id="rId9" location=".XbkUYanLfYU" display="https://www.nrcresearchpress.com/doi/10.1139/cjm-2014-0579#.XbkUYanLfYU" xr:uid="{787D25AD-74DB-EC42-8D54-EC099EEB4BD6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>